<commit_message>
sc7pro:most function is ok
Change-Id: Ida982aae494c3c18f9e2d00fc0b75e11a4f04231

Former-commit-id: 489d952b157b3c108a029db0cc4ca99616a0de75
</commit_message>
<xml_diff>
--- a/SC7PRO/config.xlsx
+++ b/SC7PRO/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27412" windowHeight="12986" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="25998" windowHeight="15015" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="218">
   <si>
     <t>Pin number</t>
   </si>
@@ -649,6 +649,12 @@
   </si>
   <si>
     <t>PMIC_OUTB</t>
+  </si>
+  <si>
+    <t>CHIP_ASSERT_N</t>
+  </si>
+  <si>
+    <t>CHIP_DEASSERT_N</t>
   </si>
   <si>
     <t>version number</t>
@@ -674,10 +680,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -705,16 +711,31 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -729,37 +750,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -774,26 +772,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -806,7 +788,53 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -820,39 +848,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -949,7 +955,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -961,139 +967,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1111,19 +985,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1242,6 +1248,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1266,6 +1287,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1277,6 +1307,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1299,191 +1340,156 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4367,17 +4373,17 @@
     <extLst/>
   </autoFilter>
   <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H12 H14:H49 H52:H66 H70:H72 H77:H92 H96:H97">
+      <formula1>"LOW,MEDIUM,HIGH,VERY-HIGH"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F49 F52:F66 F70:F72 F77:F92 F96:F97">
+      <formula1>"NO-PULL,PULL-UP,PULL-DOWN"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D108">
       <formula1>"INPUT,OUTPUT,AF,ANALOG,NA"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H13 G2:G49 G52:G66 G70:G72 G77:G92 G96:G97">
       <formula1>"PP,OD"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H12 H14:H49 H52:H66 H70:H72 H77:H92 H96:H97">
-      <formula1>"LOW,MEDIUM,HIGH,VERY-HIGH"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F49 F52:F66 F70:F72 F77:F92 F96:F97">
-      <formula1>"NO-PULL,PULL-UP,PULL-DOWN"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="A1 E1:I1 E36 J38 E49 E96 E2:E4 E8:E10 E12:E14 E17:E33 E38:E47 E52:E65 E70:E71 E77:E91 I2:I49 I52:I66 I70:I72 I77:I92 I96:I97"/>
   </dataValidations>
@@ -4390,10 +4396,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.70992366412214" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -4972,13 +4978,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="12" t="s">
-        <v>19</v>
+        <v>210</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>19</v>
+        <v>210</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D41" s="3">
         <v>0</v>
@@ -4986,24 +4992,24 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="12" t="s">
-        <v>184</v>
+        <v>211</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>184</v>
+        <v>211</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D42" s="3">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>172</v>
+      <c r="A43" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>207</v>
@@ -5014,10 +5020,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="12" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>207</v>
@@ -5028,10 +5034,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="12" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>207</v>
@@ -5042,106 +5048,22 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>207</v>
       </c>
       <c r="D46" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D47" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D48" s="3">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D49" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D50" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D51" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D52" s="3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="D2:D20"/>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C52">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C41 C42 C2:C40 C43:C46">
       <formula1>"ENABLE,FUNCTION,CHECK"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5172,22 +5094,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>